<commit_message>
Added feature to force overwrite of post - Fixes issue #17 - Also cleaned error message. Fixes #11
</commit_message>
<xml_diff>
--- a/server/routes/export/reviewTemplate-TBP.xlsx
+++ b/server/routes/export/reviewTemplate-TBP.xlsx
@@ -802,6 +802,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -810,9 +813,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1195,8 +1195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1210,10 +1210,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="72"/>
+      <c r="B1" s="69"/>
       <c r="E1" s="56" t="s">
         <v>56</v>
       </c>
@@ -1344,7 +1344,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="69" t="s">
+      <c r="A12" s="70" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="11" t="s">
@@ -1360,7 +1360,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="69"/>
+      <c r="A13" s="70"/>
       <c r="B13" s="15" t="s">
         <v>54</v>
       </c>
@@ -1372,7 +1372,7 @@
       <c r="F13" s="16"/>
     </row>
     <row r="14" spans="1:26" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="69" t="s">
+      <c r="A14" s="70" t="s">
         <v>18</v>
       </c>
       <c r="B14" s="17" t="s">
@@ -1386,7 +1386,7 @@
       <c r="F14" s="21"/>
     </row>
     <row r="15" spans="1:26" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="69"/>
+      <c r="A15" s="70"/>
       <c r="B15" s="19" t="s">
         <v>20</v>
       </c>
@@ -1400,7 +1400,7 @@
       <c r="F15" s="21"/>
     </row>
     <row r="16" spans="1:26" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="69"/>
+      <c r="A16" s="70"/>
       <c r="B16" s="19" t="s">
         <v>22</v>
       </c>
@@ -1412,7 +1412,7 @@
       <c r="F16" s="21"/>
     </row>
     <row r="17" spans="1:6" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="69"/>
+      <c r="A17" s="70"/>
       <c r="B17" s="15" t="s">
         <v>23</v>
       </c>
@@ -1424,7 +1424,7 @@
       <c r="F17" s="21"/>
     </row>
     <row r="18" spans="1:6" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="70" t="s">
+      <c r="A18" s="71" t="s">
         <v>24</v>
       </c>
       <c r="B18" s="23" t="s">
@@ -1438,7 +1438,7 @@
       <c r="F18" s="13"/>
     </row>
     <row r="19" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="70"/>
+      <c r="A19" s="71"/>
       <c r="B19" s="23" t="s">
         <v>26</v>
       </c>
@@ -1450,7 +1450,7 @@
       <c r="F19" s="21"/>
     </row>
     <row r="20" spans="1:6" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="70"/>
+      <c r="A20" s="71"/>
       <c r="B20" s="24" t="s">
         <v>27</v>
       </c>
@@ -1462,7 +1462,7 @@
       <c r="F20" s="21"/>
     </row>
     <row r="21" spans="1:6" ht="87.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="69" t="s">
+      <c r="A21" s="70" t="s">
         <v>28</v>
       </c>
       <c r="B21" s="26" t="s">
@@ -1478,7 +1478,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="69"/>
+      <c r="A22" s="70"/>
       <c r="B22" s="26" t="s">
         <v>30</v>
       </c>
@@ -1490,7 +1490,7 @@
       <c r="F22" s="16"/>
     </row>
     <row r="23" spans="1:6" ht="43.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="69" t="s">
+      <c r="A23" s="70" t="s">
         <v>31</v>
       </c>
       <c r="B23" s="33" t="s">
@@ -1504,7 +1504,7 @@
       <c r="F23" s="13"/>
     </row>
     <row r="24" spans="1:6" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="69"/>
+      <c r="A24" s="70"/>
       <c r="B24" s="28" t="s">
         <v>32</v>
       </c>
@@ -1516,7 +1516,7 @@
       <c r="F24" s="21"/>
     </row>
     <row r="25" spans="1:6" ht="47.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="69"/>
+      <c r="A25" s="70"/>
       <c r="B25" s="64" t="s">
         <v>68</v>
       </c>
@@ -1528,7 +1528,7 @@
       <c r="F25" s="21"/>
     </row>
     <row r="26" spans="1:6" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="69"/>
+      <c r="A26" s="70"/>
       <c r="B26" s="65" t="s">
         <v>46</v>
       </c>
@@ -1554,7 +1554,7 @@
       <c r="F27" s="21"/>
     </row>
     <row r="28" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="70" t="s">
+      <c r="A28" s="71" t="s">
         <v>35</v>
       </c>
       <c r="B28" s="32" t="s">
@@ -1568,7 +1568,7 @@
       <c r="F28" s="13"/>
     </row>
     <row r="29" spans="1:6" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="70"/>
+      <c r="A29" s="71"/>
       <c r="B29" s="29" t="s">
         <v>37</v>
       </c>
@@ -1580,7 +1580,7 @@
       <c r="F29" s="16"/>
     </row>
     <row r="30" spans="1:6" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="69" t="s">
+      <c r="A30" s="70" t="s">
         <v>38</v>
       </c>
       <c r="B30" s="33" t="s">
@@ -1594,7 +1594,7 @@
       <c r="F30" s="13"/>
     </row>
     <row r="31" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="69"/>
+      <c r="A31" s="70"/>
       <c r="B31" s="26" t="s">
         <v>39</v>
       </c>
@@ -1606,7 +1606,7 @@
       <c r="F31" s="21"/>
     </row>
     <row r="32" spans="1:6" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="69"/>
+      <c r="A32" s="70"/>
       <c r="B32" s="26" t="s">
         <v>40</v>
       </c>
@@ -1618,7 +1618,7 @@
       <c r="F32" s="21"/>
     </row>
     <row r="33" spans="1:6" ht="75.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="69"/>
+      <c r="A33" s="70"/>
       <c r="B33" s="35" t="s">
         <v>63</v>
       </c>
@@ -1645,10 +1645,10 @@
     </row>
     <row r="35" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="62"/>
-      <c r="B35" s="71" t="s">
+      <c r="B35" s="72" t="s">
         <v>42</v>
       </c>
-      <c r="C35" s="71"/>
+      <c r="C35" s="72"/>
       <c r="D35" s="36"/>
       <c r="E35" s="46"/>
       <c r="F35" s="48"/>

</xml_diff>